<commit_message>
updated lab02 excel file
</commit_message>
<xml_diff>
--- a/cmir3097/Docs/Lab02/Lab02_BBT_TCs_Form3testeri.xlsx
+++ b/cmir3097/Docs/Lab02/Lab02_BBT_TCs_Form3testeri.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B00B2AD-EE72-4B13-9BF2-2046B1C450FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B83CAA-FA70-4635-9046-53E67B6F9CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1020" windowWidth="19116" windowHeight="11100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="160">
   <si>
     <t>VVSS, Info Romana, 2023-2024</t>
   </si>
@@ -474,9 +474,6 @@
     <t>hour &gt;= 24</t>
   </si>
   <si>
-    <t>minute &gt; 60</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -534,12 +531,6 @@
     <t>1.01 time = "", len = 0</t>
   </si>
   <si>
-    <t>1.03 time = "1…..0", len = 255</t>
-  </si>
-  <si>
-    <t>1.04 time = "1…..01" len = 256</t>
-  </si>
-  <si>
     <t>2.01. hour = -1</t>
   </si>
   <si>
@@ -591,12 +582,6 @@
     <t>error</t>
   </si>
   <si>
-    <t>1.02, 2.03,3.02,4.03</t>
-  </si>
-  <si>
-    <t>1.02 time = "0:1", len = 3</t>
-  </si>
-  <si>
     <t>"0:1"</t>
   </si>
   <si>
@@ -712,6 +697,27 @@
   </si>
   <si>
     <t>yes - first time</t>
+  </si>
+  <si>
+    <t>minute &gt;= 60</t>
+  </si>
+  <si>
+    <t>1.03 time = "", len = 2</t>
+  </si>
+  <si>
+    <t>1.02 time = "", len = 1</t>
+  </si>
+  <si>
+    <t>1.04 time = "0:1", len = 254</t>
+  </si>
+  <si>
+    <t>1.04 time = "1…..0", len = 255</t>
+  </si>
+  <si>
+    <t>1.05 time = "1…..01" len = 256</t>
+  </si>
+  <si>
+    <t>2.03,3.02,4.03</t>
   </si>
 </sst>
 </file>
@@ -1517,6 +1523,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1532,6 +1541,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1574,44 +1622,28 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1634,9 +1666,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1646,25 +1675,77 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1677,81 +1758,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2076,12 +2082,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="53"/>
       <c r="H1" s="43" t="s">
         <v>1</v>
       </c>
@@ -2089,11 +2095,11 @@
       <c r="J1" s="43"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -2256,21 +2262,21 @@
     </row>
     <row r="24" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C26" s="42"/>
@@ -2294,7 +2300,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2312,38 +2318,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="73"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="G5" s="61" t="s">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="G5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
@@ -2358,50 +2364,50 @@
       <c r="E6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="62" t="s">
+      <c r="G6" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="74" t="s">
+      <c r="H6" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="77" t="s">
+      <c r="I6" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="78"/>
-      <c r="K6" s="76" t="s">
+      <c r="J6" s="66"/>
+      <c r="K6" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="76"/>
+      <c r="L6" s="64"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="68" t="s">
         <v>70</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="75"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="63"/>
       <c r="I7" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="79"/>
+      <c r="L7" s="67"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="54"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>72</v>
@@ -2410,24 +2416,24 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="L8" s="73"/>
+      <c r="L8" s="61"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="68" t="s">
         <v>74</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2438,24 +2444,24 @@
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K9" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="L9" s="73"/>
+        <v>83</v>
+      </c>
+      <c r="K9" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="61"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>77</v>
@@ -2464,24 +2470,24 @@
         <v>3</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I10" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="29" t="s">
+      <c r="K10" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="K10" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="L10" s="65"/>
+      <c r="L10" s="79"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="68" t="s">
         <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -2492,30 +2498,30 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="67"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="81"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="54"/>
+      <c r="C12" s="68"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="69"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="56"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="69" t="s">
         <v>73</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -2526,30 +2532,30 @@
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="69"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="56"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="56"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="71"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="58"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="68" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="4"/>
@@ -2558,28 +2564,28 @@
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="71"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="58"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
-      <c r="K16" s="70"/>
-      <c r="L16" s="71"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="58"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="68" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="4"/>
@@ -2588,28 +2594,28 @@
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="71"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="58"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="54"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="19"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="71"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="58"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="68" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="4"/>
@@ -2618,14 +2624,14 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="71"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="58"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="54"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
@@ -2633,24 +2639,11 @@
       <c r="D22" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K7:L7"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C7:C8"/>
@@ -2667,6 +2660,19 @@
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2677,10 +2683,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:N28"/>
+  <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="G5:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2701,40 +2707,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="73"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
     </row>
     <row r="6" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -2747,554 +2753,586 @@
         <v>32</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="G6" s="62" t="s">
+      <c r="G6" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="74" t="s">
+      <c r="J6" s="62" t="s">
         <v>38</v>
       </c>
       <c r="K6" s="47" t="s">
         <v>25</v>
       </c>
       <c r="L6" s="48"/>
-      <c r="M6" s="94" t="s">
+      <c r="M6" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="95"/>
+      <c r="N6" s="86"/>
     </row>
     <row r="7" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="55">
+      <c r="B7" s="69">
         <v>1</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="69" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="E7" s="10"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="95" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="98"/>
+    </row>
+    <row r="8" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="99"/>
+    </row>
+    <row r="9" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="99"/>
+    </row>
+    <row r="10" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="99"/>
+    </row>
+    <row r="11" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="96"/>
+      <c r="N11" s="99"/>
+    </row>
+    <row r="12" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="99"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="69">
+        <v>2</v>
+      </c>
+      <c r="C13" s="92" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="85" t="s">
-        <v>79</v>
-      </c>
-      <c r="L7" s="74" t="s">
-        <v>95</v>
-      </c>
-      <c r="M7" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="89"/>
-    </row>
-    <row r="8" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="86"/>
-      <c r="N8" s="90"/>
-    </row>
-    <row r="9" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="46" t="s">
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="100"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="91"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="90"/>
-    </row>
-    <row r="10" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="90"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="55">
-        <v>2</v>
-      </c>
-      <c r="C11" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="87"/>
-      <c r="N11" s="91"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="81"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G12" s="20">
+      <c r="G14" s="20">
         <v>1</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H14" s="17">
         <v>1.01</v>
-      </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="M12" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="N12" s="65"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="81"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="45">
-        <v>2</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="L13" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="M13" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="N13" s="65"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="81"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="20">
-        <v>3</v>
-      </c>
-      <c r="H14" s="17">
-        <v>1.04</v>
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="28" t="s">
-        <v>122</v>
+      <c r="K14" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="M14" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="N14" s="65"/>
+        <v>80</v>
+      </c>
+      <c r="M14" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="N14" s="79"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="81"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="96" t="s">
-        <v>104</v>
-      </c>
-      <c r="G15" s="20">
-        <v>4</v>
-      </c>
-      <c r="H15" s="17">
-        <v>2.04</v>
+      <c r="B15" s="91"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="45">
+        <v>2</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>159</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="28" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="L15" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="M15" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="N15" s="65"/>
+        <v>115</v>
+      </c>
+      <c r="M15" s="78" t="s">
+        <v>116</v>
+      </c>
+      <c r="N15" s="79"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="56"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="97"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="G16" s="20">
-        <v>5</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>126</v>
+        <v>3</v>
+      </c>
+      <c r="H16" s="17">
+        <v>1.05</v>
       </c>
       <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="J16" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="K16" s="28" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="L16" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="M16" s="64" t="s">
-        <v>128</v>
-      </c>
-      <c r="N16" s="65"/>
+        <v>118</v>
+      </c>
+      <c r="M16" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="N16" s="79"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="55">
-        <v>3</v>
-      </c>
-      <c r="C17" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17" s="45">
-        <v>6</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>129</v>
+      <c r="B17" s="91"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="88" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="20">
+        <v>4</v>
+      </c>
+      <c r="H17" s="17">
+        <v>2.04</v>
       </c>
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="28" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L17" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="M17" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="N17" s="65"/>
+        <v>119</v>
+      </c>
+      <c r="M17" s="78" t="s">
+        <v>127</v>
+      </c>
+      <c r="N17" s="79"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="B18" s="70"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="89"/>
       <c r="G18" s="20">
-        <v>7</v>
-      </c>
-      <c r="H18" s="17">
-        <v>2.0499999999999998</v>
+        <v>5</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>121</v>
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
-      <c r="K18" s="29" t="s">
-        <v>133</v>
+      <c r="K18" s="28" t="s">
+        <v>122</v>
       </c>
       <c r="L18" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="M18" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="N18" s="65"/>
+        <v>120</v>
+      </c>
+      <c r="M18" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="N18" s="79"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
+      <c r="B19" s="69">
+        <v>3</v>
+      </c>
+      <c r="C19" s="69" t="s">
+        <v>92</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="20">
-        <v>8</v>
-      </c>
-      <c r="H19" s="17">
-        <v>2.0099999999999998</v>
+        <v>102</v>
+      </c>
+      <c r="G19" s="45">
+        <v>6</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
-      <c r="K19" s="29" t="s">
-        <v>85</v>
+      <c r="K19" s="28" t="s">
+        <v>125</v>
       </c>
       <c r="L19" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="M19" s="64" t="s">
-        <v>128</v>
-      </c>
-      <c r="N19" s="65"/>
+        <v>115</v>
+      </c>
+      <c r="M19" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="N19" s="79"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
       <c r="D20" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G20" s="20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H20" s="17">
-        <v>3.05</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="K20" s="29" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="L20" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="M20" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="N20" s="65"/>
+        <v>129</v>
+      </c>
+      <c r="M20" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="N20" s="79"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="98" t="s">
-        <v>109</v>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="G21" s="20">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H21" s="17">
-        <v>4.01</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="K21" s="29" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="L21" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="M21" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="N21" s="65"/>
+        <v>120</v>
+      </c>
+      <c r="M21" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="N21" s="79"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="99"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="G22" s="20">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H22" s="17">
-        <v>4.05</v>
+        <v>3.05</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="29" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="M22" s="64" t="s">
-        <v>139</v>
-      </c>
-      <c r="N22" s="65"/>
+        <v>129</v>
+      </c>
+      <c r="M22" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="N22" s="79"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="55">
-        <v>4</v>
-      </c>
-      <c r="C23" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>110</v>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="82" t="s">
+        <v>106</v>
       </c>
       <c r="G23" s="20">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H23" s="17">
-        <v>4.0599999999999996</v>
+        <v>4.01</v>
       </c>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="29" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="L23" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="M23" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="N23" s="65"/>
+        <v>131</v>
+      </c>
+      <c r="M23" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="N23" s="79"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="81"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="83"/>
       <c r="G24" s="20">
-        <v>13</v>
-      </c>
-      <c r="H24" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="H24" s="17">
+        <v>4.05</v>
+      </c>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="65"/>
+      <c r="K24" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="L24" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="M24" s="78" t="s">
+        <v>134</v>
+      </c>
+      <c r="N24" s="79"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="81"/>
-      <c r="C25" s="83"/>
+      <c r="B25" s="69">
+        <v>4</v>
+      </c>
+      <c r="C25" s="92" t="s">
+        <v>93</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G25" s="20">
-        <v>14</v>
-      </c>
-      <c r="H25" s="17"/>
+        <v>12</v>
+      </c>
+      <c r="H25" s="17">
+        <v>4.0599999999999996</v>
+      </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="65"/>
+      <c r="K25" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="M25" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="N25" s="79"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="81"/>
-      <c r="C26" s="83"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="93"/>
       <c r="D26" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G26" s="20">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="29"/>
       <c r="L26" s="29"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="65"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="79"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="81"/>
-      <c r="C27" s="83"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="93"/>
       <c r="D27" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G27" s="20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="65"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="79"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="56"/>
-      <c r="C28" s="84"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="93"/>
       <c r="D28" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G28" s="20">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="16"/>
       <c r="J28" s="16"/>
       <c r="K28" s="29"/>
       <c r="L28" s="29"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="65"/>
+      <c r="M28" s="78"/>
+      <c r="N28" s="79"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="91"/>
+      <c r="C29" s="93"/>
+      <c r="D29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="20">
+        <v>16</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="79"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="70"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="20">
+        <v>17</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="C25:C30"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="K7:K13"/>
+    <mergeCell ref="L7:L13"/>
+    <mergeCell ref="M7:N13"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G6:G13"/>
+    <mergeCell ref="I6:I13"/>
+    <mergeCell ref="J6:J13"/>
+    <mergeCell ref="B13:B18"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="M16:N16"/>
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="H6:H13"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G6:G11"/>
-    <mergeCell ref="I6:I11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="M7:N11"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="M25:N25"/>
     <mergeCell ref="M26:N26"/>
     <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M19:N19"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3309,8 +3347,8 @@
   </sheetPr>
   <dimension ref="B1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F21" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3322,57 +3360,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="F4" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="76" t="s">
+      <c r="G4" s="66"/>
+      <c r="H4" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="76"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="108"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="100"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="125"/>
       <c r="F5" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>27</v>
@@ -3385,7 +3423,7 @@
       <c r="B6" s="21">
         <v>1</v>
       </c>
-      <c r="C6" s="105" t="s">
+      <c r="C6" s="110" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="26" t="s">
@@ -3395,16 +3433,16 @@
         <v>29</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
@@ -3412,9 +3450,9 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="106"/>
+      <c r="C7" s="111"/>
       <c r="D7" s="27" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>29</v>
@@ -3423,13 +3461,13 @@
         <v>30</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
@@ -3437,7 +3475,7 @@
         <f t="shared" ref="B8:B12" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="106"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="27" t="s">
         <v>49</v>
       </c>
@@ -3445,16 +3483,16 @@
         <v>29</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
@@ -3462,24 +3500,24 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="106"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="27" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" s="128" t="s">
-        <v>148</v>
-      </c>
-      <c r="G9" s="128" t="s">
-        <v>134</v>
-      </c>
-      <c r="H9" s="128" t="s">
-        <v>149</v>
+        <v>136</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>144</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
@@ -3487,7 +3525,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="106"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="27" t="s">
         <v>29</v>
       </c>
@@ -3495,16 +3533,16 @@
         <v>50</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
@@ -3512,24 +3550,24 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="106"/>
+      <c r="C11" s="111"/>
       <c r="D11" s="27" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
@@ -3537,24 +3575,24 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="107"/>
+      <c r="C12" s="112"/>
       <c r="D12" s="27" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
@@ -3579,98 +3617,98 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="118"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="106"/>
       <c r="G16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="116" t="s">
+      <c r="H16" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="119"/>
-      <c r="J16" s="117"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="116" t="s">
+      <c r="I16" s="104"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="N16" s="119"/>
-      <c r="O16" s="117"/>
-      <c r="P16" s="118"/>
+      <c r="N16" s="104"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="106"/>
     </row>
     <row r="17" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="112" t="s">
+      <c r="B17" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="113" t="s">
+      <c r="C17" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="114" t="s">
+      <c r="D17" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="114" t="s">
+      <c r="E17" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="115" t="s">
+      <c r="F17" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="124" t="s">
+      <c r="G17" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="120" t="s">
+      <c r="H17" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="121"/>
-      <c r="J17" s="114" t="s">
+      <c r="I17" s="120"/>
+      <c r="J17" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="K17" s="114" t="s">
+      <c r="K17" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="L17" s="115" t="s">
+      <c r="L17" s="101" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="126" t="s">
+      <c r="M17" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="N17" s="114" t="s">
+      <c r="N17" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="O17" s="114" t="s">
+      <c r="O17" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="P17" s="115" t="s">
+      <c r="P17" s="101" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="112"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="115"/>
-      <c r="G18" s="125"/>
-      <c r="H18" s="122"/>
-      <c r="I18" s="123"/>
-      <c r="J18" s="114"/>
-      <c r="K18" s="114"/>
-      <c r="L18" s="115"/>
-      <c r="M18" s="127"/>
-      <c r="N18" s="114"/>
-      <c r="O18" s="114"/>
-      <c r="P18" s="115"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="121"/>
+      <c r="I18" s="122"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="102"/>
+      <c r="L18" s="101"/>
+      <c r="M18" s="108"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="102"/>
+      <c r="P18" s="101"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="36" t="s">
@@ -3691,10 +3729,10 @@
       <c r="G19" s="38">
         <v>4</v>
       </c>
-      <c r="H19" s="110" t="s">
-        <v>157</v>
-      </c>
-      <c r="I19" s="111"/>
+      <c r="H19" s="115" t="s">
+        <v>152</v>
+      </c>
+      <c r="I19" s="116"/>
       <c r="J19" s="2">
         <v>3</v>
       </c>
@@ -3705,7 +3743,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="37" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="N19" s="2">
         <v>4</v>
@@ -3719,12 +3757,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B3:I3"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="C6:C12"/>
     <mergeCell ref="B4:B5"/>
@@ -3741,12 +3779,12 @@
     <mergeCell ref="H17:I18"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="K17:K18"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="N17:N18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3761,15 +3799,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -3913,6 +3942,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
   <ds:schemaRefs>
@@ -3923,14 +3961,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153A5999-B236-48B1-944C-C5EB94545735}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3946,4 +3976,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>